<commit_message>
Added : Sign up of Facebook application
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/facebook/scenarios/fb_scenarios.xlsx
+++ b/src/main/java/com/qa/facebook/scenarios/fb_scenarios.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="signup" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>test step</t>
   </si>
   <si>
-    <t>locator</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -51,27 +48,18 @@
     <t xml:space="preserve">enter email or phone number </t>
   </si>
   <si>
-    <t>name=email</t>
-  </si>
-  <si>
     <t>sendKeys</t>
   </si>
   <si>
     <t>enter password</t>
   </si>
   <si>
-    <t>name=password</t>
-  </si>
-  <si>
     <t>test@12345</t>
   </si>
   <si>
     <t>click on login button</t>
   </si>
   <si>
-    <t>name=login</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -84,7 +72,55 @@
     <t>verify sign up link</t>
   </si>
   <si>
-    <t>linkText=Create New Account</t>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>locatorValue</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>Create New Account</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//*[name()='path' and contains(@d,'M15 35.8C6')]</t>
+  </si>
+  <si>
+    <t>verify home logo</t>
+  </si>
+  <si>
+    <t>get home page title</t>
+  </si>
+  <si>
+    <t>isDisplayed</t>
+  </si>
+  <si>
+    <t>//title[contains(text(),'Facebook')]</t>
+  </si>
+  <si>
+    <t>getText</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -447,193 +483,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="29.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" s="2">
+        <v>8109555221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2">
-        <v>8109555221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
+      <c r="E9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>